<commit_message>
plots and classification update
</commit_message>
<xml_diff>
--- a/xlslist/Acc_other_class.xlsx
+++ b/xlslist/Acc_other_class.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -520,19 +520,19 @@
         <v>6089</v>
       </c>
       <c r="E3" t="n">
-        <v>66.42036124794745</v>
+        <v>67.32348111658456</v>
       </c>
       <c r="F3" t="n">
-        <v>72.66009852216749</v>
+        <v>74.13793103448276</v>
       </c>
       <c r="G3" t="n">
-        <v>71.92118226600985</v>
+        <v>72.41379310344827</v>
       </c>
       <c r="H3" t="n">
-        <v>83.70279146141215</v>
+        <v>84.40065681444992</v>
       </c>
       <c r="I3" t="n">
-        <v>87.72577996715928</v>
+        <v>87.25451559934319</v>
       </c>
     </row>
     <row r="4">
@@ -551,19 +551,19 @@
         <v>5799</v>
       </c>
       <c r="E4" t="n">
-        <v>74.95689655172414</v>
+        <v>75.94827586206897</v>
       </c>
       <c r="F4" t="n">
-        <v>79.31034482758621</v>
+        <v>80.94827586206897</v>
       </c>
       <c r="G4" t="n">
-        <v>79.05172413793103</v>
+        <v>81.37931034482759</v>
       </c>
       <c r="H4" t="n">
-        <v>87.37068965517241</v>
+        <v>88.70689655172413</v>
       </c>
       <c r="I4" t="n">
-        <v>92.58620689655173</v>
+        <v>92.57413793103451</v>
       </c>
     </row>
     <row r="5">
@@ -582,19 +582,19 @@
         <v>5788</v>
       </c>
       <c r="E5" t="n">
-        <v>71.80483592400691</v>
+        <v>73.48877374784111</v>
       </c>
       <c r="F5" t="n">
-        <v>76.94300518134715</v>
+        <v>78.75647668393782</v>
       </c>
       <c r="G5" t="n">
-        <v>76.46804835924007</v>
+        <v>78.41105354058722</v>
       </c>
       <c r="H5" t="n">
-        <v>84.41278065630398</v>
+        <v>85.49222797927462</v>
       </c>
       <c r="I5" t="n">
-        <v>90.50086355785838</v>
+        <v>90.95682210708118</v>
       </c>
     </row>
     <row r="6">
@@ -613,19 +613,19 @@
         <v>5778</v>
       </c>
       <c r="E6" t="n">
-        <v>59.51557093425605</v>
+        <v>61.5916955017301</v>
       </c>
       <c r="F6" t="n">
-        <v>54.88754325259516</v>
+        <v>56.74740484429066</v>
       </c>
       <c r="G6" t="n">
-        <v>56.18512110726643</v>
+        <v>55.88235294117647</v>
       </c>
       <c r="H6" t="n">
-        <v>66.91176470588235</v>
+        <v>71.280276816609</v>
       </c>
       <c r="I6" t="n">
-        <v>82.48269896193771</v>
+        <v>83.4134948096886</v>
       </c>
     </row>
     <row r="7">
@@ -638,25 +638,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" t="n">
-        <v>5854</v>
+        <v>5845</v>
       </c>
       <c r="E7" t="n">
-        <v>49.5730145175064</v>
+        <v>51.15483319076134</v>
       </c>
       <c r="F7" t="n">
-        <v>51.66524338172502</v>
+        <v>52.95124037639007</v>
       </c>
       <c r="G7" t="n">
-        <v>46.49871904355252</v>
+        <v>47.56201881950385</v>
       </c>
       <c r="H7" t="n">
-        <v>61.52860802732707</v>
+        <v>63.47305389221557</v>
       </c>
       <c r="I7" t="n">
-        <v>79.54739538855678</v>
+        <v>80.22754491017963</v>
       </c>
     </row>
     <row r="8">
@@ -669,25 +669,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" t="n">
-        <v>5847</v>
+        <v>5838</v>
       </c>
       <c r="E8" t="n">
-        <v>48.61051731509193</v>
+        <v>48.88698630136986</v>
       </c>
       <c r="F8" t="n">
-        <v>54.9807610089782</v>
+        <v>55.65068493150685</v>
       </c>
       <c r="G8" t="n">
-        <v>47.96921761436511</v>
+        <v>48.88698630136986</v>
       </c>
       <c r="H8" t="n">
-        <v>58.9140658401026</v>
+        <v>60.61643835616438</v>
       </c>
       <c r="I8" t="n">
-        <v>78.28131680205216</v>
+        <v>79.62157534246576</v>
       </c>
     </row>
     <row r="9">
@@ -700,25 +700,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="D9" t="n">
-        <v>6030</v>
+        <v>5990</v>
       </c>
       <c r="E9" t="n">
-        <v>34.99170812603649</v>
+        <v>36.64440734557596</v>
       </c>
       <c r="F9" t="n">
-        <v>42.66169154228855</v>
+        <v>43.23873121869783</v>
       </c>
       <c r="G9" t="n">
-        <v>27.32172470978441</v>
+        <v>27.04507512520868</v>
       </c>
       <c r="H9" t="n">
-        <v>40.09121061359867</v>
+        <v>42.98831385642738</v>
       </c>
       <c r="I9" t="n">
-        <v>72.18076285240464</v>
+        <v>74.45909849749583</v>
       </c>
     </row>
     <row r="10">
@@ -731,25 +731,25 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>515</v>
+        <v>360</v>
       </c>
       <c r="D10" t="n">
-        <v>5092</v>
+        <v>4673</v>
       </c>
       <c r="E10" t="n">
-        <v>38.53706431026019</v>
+        <v>44.59893048128342</v>
       </c>
       <c r="F10" t="n">
-        <v>28.96416298478155</v>
+        <v>36.79144385026738</v>
       </c>
       <c r="G10" t="n">
-        <v>16.3966617574865</v>
+        <v>18.82352941176471</v>
       </c>
       <c r="H10" t="n">
-        <v>14.48208149239077</v>
+        <v>17.64705882352941</v>
       </c>
       <c r="I10" t="n">
-        <v>60.23564064801178</v>
+        <v>68.71229946524065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>